<commit_message>
tes case id new row added
</commit_message>
<xml_diff>
--- a/testcasesOpenCart.xlsx
+++ b/testcasesOpenCart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rovan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Newfolder\gitrepo\gitlocal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3941" uniqueCount="2075">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3942" uniqueCount="2076">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -8006,6 +8006,9 @@
     <t>Email Address - xyzabc123@gmail.com
 Password - 
 241001</t>
+  </si>
+  <si>
+    <t>TC_SPO_017</t>
   </si>
 </sst>
 </file>
@@ -20443,10 +20446,10 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20943,6 +20946,11 @@
       <c r="I18" s="15"/>
       <c r="J18" s="16"/>
       <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>2075</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>